<commit_message>
added remarks and latest changes
</commit_message>
<xml_diff>
--- a/studentdata.xlsx
+++ b/studentdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="562">
   <si>
     <t>Name</t>
   </si>
@@ -1702,6 +1702,9 @@
   </si>
   <si>
     <t>Distrcit</t>
+  </si>
+  <si>
+    <t>School of Computing and Informatics</t>
   </si>
 </sst>
 </file>
@@ -1711,7 +1714,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1746,6 +1749,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF575151"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1769,7 +1778,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1809,6 +1818,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2083,7 +2093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2093,8 +2103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BO39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AU7" sqref="AU7"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2477,6 +2487,9 @@
       <c r="BD2" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="BG2" s="15" t="s">
+        <v>561</v>
+      </c>
       <c r="BH2" s="5" t="s">
         <v>505</v>
       </c>
@@ -2540,7 +2553,7 @@
         <v>168</v>
       </c>
       <c r="Q3" s="1">
-        <v>33130</v>
+        <v>33648</v>
       </c>
       <c r="R3" t="s">
         <v>125</v>
@@ -2680,7 +2693,7 @@
         <v>30</v>
       </c>
       <c r="Q4" s="1">
-        <v>33131</v>
+        <v>34653</v>
       </c>
       <c r="R4" t="s">
         <v>125</v>
@@ -2820,7 +2833,7 @@
         <v>30</v>
       </c>
       <c r="Q5" s="1">
-        <v>33132</v>
+        <v>25857</v>
       </c>
       <c r="R5" t="s">
         <v>125</v>
@@ -2960,7 +2973,7 @@
         <v>30</v>
       </c>
       <c r="Q6" s="1">
-        <v>33133</v>
+        <v>31763</v>
       </c>
       <c r="R6" t="s">
         <v>125</v>
@@ -3342,7 +3355,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="9" spans="1:67" ht="25.5">
+    <row r="9" spans="1:67">
       <c r="B9" s="3" t="s">
         <v>69</v>
       </c>

</xml_diff>